<commit_message>
StaticData TypeTest 추가 (#70)
</commit_message>
<xml_diff>
--- a/StaticData/__TestStaticData/Data01.xlsx
+++ b/StaticData/__TestStaticData/Data01.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\gitProject\Playground\StaticData\MultiExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\gitProject\Playground\StaticData\__TestStaticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FB9502-9290-42E5-9FD3-45065EDBE929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370D1046-1D3A-4A05-B293-945BD7C91E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="2670" windowWidth="28800" windowHeight="15900" activeTab="1" xr2:uid="{8EF6EFD5-36D8-4DAA-83AD-49C34620FFDD}"/>
+    <workbookView xWindow="6960" yWindow="14085" windowWidth="28800" windowHeight="15900" activeTab="2" xr2:uid="{8EF6EFD5-36D8-4DAA-83AD-49C34620FFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="TargetTest" sheetId="6" r:id="rId1"/>
     <sheet name="ClassListTest" sheetId="9" r:id="rId2"/>
+    <sheet name="TypeTest" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,6 +142,120 @@
   <si>
     <t>Grade3</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISO 8601 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1일 10초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UIntValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShortValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LongValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FloatValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DoubleValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CharValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StringValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnumValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DateTimeValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeSpanValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-1.7976931348623157E+308</t>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MinValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>0001-01-01T00:00:00Z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-10675199.02:48:05.4775808</t>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㅋㅋㅋ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1986-05-26T01:05:00+09:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.00:00:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.7976931348623157E+308</t>
+  </si>
+  <si>
+    <t>0xFFFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>9999-12-31T23:59:59Z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10675199.02:48:05.4775807</t>
   </si>
 </sst>
 </file>
@@ -186,8 +301,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -623,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BF872F-4979-41FA-BD82-57FC6B4507C3}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -751,4 +869,187 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EA9AE3-2BD2-4FC9-B7E0-7E4D14956374}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>-2147483648</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>-32768</v>
+      </c>
+      <c r="F11">
+        <v>-9.2233720368547697E+18</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-3.4028234999999999E+38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1001</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>3.1415920000000002</v>
+      </c>
+      <c r="H12">
+        <v>3.1415926535896999</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2147483647</v>
+      </c>
+      <c r="D13">
+        <v>4294967295</v>
+      </c>
+      <c r="E13">
+        <v>32767</v>
+      </c>
+      <c r="F13">
+        <v>9.2233720368547697E+18</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3.4028234999999999E+38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
StaticData 외래키 테스트 (#73)
</commit_message>
<xml_diff>
--- a/StaticData/__TestStaticData/Data01.xlsx
+++ b/StaticData/__TestStaticData/Data01.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\gitProject\Playground\StaticData\__TestStaticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0EC62B-9F5B-46B3-8335-308F745D6D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A83040C-31E7-4710-B47E-24AD86DFAABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12645" yWindow="4035" windowWidth="24885" windowHeight="13125" activeTab="3" xr2:uid="{8EF6EFD5-36D8-4DAA-83AD-49C34620FFDD}"/>
+    <workbookView xWindow="6990" yWindow="1470" windowWidth="24885" windowHeight="13125" activeTab="4" xr2:uid="{8EF6EFD5-36D8-4DAA-83AD-49C34620FFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="TargetTest" sheetId="6" r:id="rId1"/>
     <sheet name="ClassListTest" sheetId="9" r:id="rId2"/>
     <sheet name="TypeTest" sheetId="10" r:id="rId3"/>
     <sheet name="GroupTest" sheetId="11" r:id="rId4"/>
+    <sheet name="MultiForeignTest" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -264,6 +265,26 @@
   </si>
   <si>
     <t>C2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중첩 외래키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1067,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4843BF10-671C-4C60-B9F6-25E8F4080ECF}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1106,4 +1127,58 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6FC92AE-576B-4BB5-AFEA-655BE6453345}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <v>1001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>5001</v>
+      </c>
+      <c r="E7">
+        <v>1003</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>